<commit_message>
Updated #8 with URL
</commit_message>
<xml_diff>
--- a/docs/Evidence/Attachment E Approach Criteria Evidence NorthropGrumman.xlsx
+++ b/docs/Evidence/Attachment E Approach Criteria Evidence NorthropGrumman.xlsx
@@ -104,24 +104,6 @@
     <t>Using our Agile framework, which is built upon Scrum, Extreme Programming, and user-centered design techniques, we were able to develop the product in an iterative fashion while receiving regular, timely feedback from users and stakeholders. We conducted an initial sprint 0 as we identified the team and coordinated the infrastructure. Then we used sprint cycles of 5 hours each comprised of sprint planning, execution, and review (demo and retrospective).
 Digital Playbook#4 Build the service using agile and iterative practices
 URL: http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Research%20Findings/Generative_Research.pdf</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Our MedExplorer prototype was design for multiple platforms including PCs, laptops, tablets, and phones.
-Digital Playbook#2 Address the whole experience, from start to finish
-Digital Playbook#7 Bring in experienced teams
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-URL: [TODO: need screenshots and pictures for multiple platforms]</t>
-    </r>
   </si>
   <si>
     <t>Using our Agile framework, which is built upon Scrum, Extreme Programming, and user-centered design techniques, we were able to develop the product in an iterative fashion while receiving regular, timely feedback from users and stakeholders. We conducted an initial sprint 0 as we identified the team and coordinated the infrastructure. Then we used sprint cycles of 5 hours each comprised of sprint planning, execution, and review (demo and retrospective).
@@ -252,12 +234,19 @@
 http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User Centered Design/Research Findings/Focus Group2.pdf
 http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Research%20Findings/Generative_Research.pdf</t>
   </si>
+  <si>
+    <t>Our MedExplorer prototype was design for multiple platforms including PCs, laptops, tablets, and phones.
+Digital Playbook#2 Address the whole experience, from start to finish
+Digital Playbook#7 Bring in experienced teams
+URL: 
+http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Platform%20Support.md</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -276,12 +265,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -48783,7 +48766,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="2"/>
@@ -48813,7 +48796,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="2"/>
@@ -48843,7 +48826,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="2"/>
@@ -48873,7 +48856,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="2"/>
@@ -48903,7 +48886,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -48932,7 +48915,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="2"/>
@@ -48984,15 +48967,15 @@
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
     </row>
-    <row r="9" spans="1:22" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" ht="111" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>27</v>
+      <c r="C9" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="2"/>
@@ -49022,7 +49005,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="2"/>
@@ -49052,7 +49035,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="2"/>
@@ -49082,7 +49065,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="2"/>
@@ -49112,7 +49095,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="2"/>
@@ -49142,7 +49125,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="2"/>
@@ -49172,7 +49155,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="2"/>
@@ -49202,7 +49185,7 @@
         <v>18</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="2"/>
@@ -49232,7 +49215,7 @@
         <v>19</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="2"/>
@@ -49262,7 +49245,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="2"/>
@@ -49292,7 +49275,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="2"/>
@@ -49322,7 +49305,7 @@
         <v>21</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="2"/>

</xml_diff>

<commit_message>
Updated URLs to match readme evidence
</commit_message>
<xml_diff>
--- a/docs/Evidence/Attachment E Approach Criteria Evidence NorthropGrumman.xlsx
+++ b/docs/Evidence/Attachment E Approach Criteria Evidence NorthropGrumman.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
   <si>
     <t>#</t>
   </si>
@@ -101,17 +101,6 @@
     <t>assembled a multidisciplinary and collaborative team including a minimum of 5 labor categories from the Development Pool labor categories to design and develop the prototype</t>
   </si>
   <si>
-    <t>Using our Agile framework, which is built upon Scrum, Extreme Programming, and user-centered design techniques, we were able to develop the product in an iterative fashion while receiving regular, timely feedback from users and stakeholders. We conducted an initial sprint 0 as we identified the team and coordinated the infrastructure. Then we used sprint cycles of 5 hours each comprised of sprint planning, execution, and review (demo and retrospective).
-Digital Playbook#4 Build the service using agile and iterative practices
-URL: http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Research%20Findings/Generative_Research.pdf</t>
-  </si>
-  <si>
-    <t>Using our Agile framework, which is built upon Scrum, Extreme Programming, and user-centered design techniques, we were able to develop the product in an iterative fashion while receiving regular, timely feedback from users and stakeholders. We conducted an initial sprint 0 as we identified the team and coordinated the infrastructure. Then we used sprint cycles of 5 hours each comprised of sprint planning, execution, and review (demo and retrospective).
-Digital Playbook#4 Build the service using agile and iterative practices
-URL: 
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Research%20Findings/Generative_Research.pdf</t>
-  </si>
-  <si>
     <t>For our MedExplorer prototype, we used the openFDA API for Drug Labeling, Drug Enforcement Reports, and Drug Adverse Events.
 Digital Playbook#13 Default to open
 URL: 
@@ -128,24 +117,6 @@
 Digital Playbook#7 Bring in experienced teams
 URL:
 http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/MedExplorer%20Development%20Team.md</t>
-  </si>
-  <si>
-    <t>Our User Experience design team interviewed and performed user tests with a number for General Public and Clinician users. The team also met with Northrop Grumman's Clinical Advisory Group as part of our Health Division. Users participated in periodic demonstrations for feedback. Created scenarios and stories. The team gave periodic demonstrations to walk through scenarios and gather feedback. We captured feedback as user stories and added to the backlog for prioritization.
-Digital Playbook#1: Understand what people need
-URL: 
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/User%20Centered%20Design.md</t>
-  </si>
-  <si>
-    <t>Our User Centered Design approach used a number of techniques and tools, including interviews, focus groups, expectancy tests, generative research, and usability tests.
-Digital Playbook#3 Make it simple and intuitive
-URL: 
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/User%20Centered%20Design.md</t>
-  </si>
-  <si>
-    <t>Our MedExplorer used a number for modern, open source technologies, including TwitterBootstrap, AngularJS, NodeJS, ExpressJS, Docker, MongoDB, Jenkins and Zabbix.
-Digital Playbook#8 Choose a modern technology stack
-URL: 
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/License.md#open-source-third-party-software-licenses</t>
   </si>
   <si>
     <t xml:space="preserve">Our development wrote unit tests for their code and was part of the team's definition of done.
@@ -202,19 +173,6 @@
     </r>
   </si>
   <si>
-    <t>Our development team used Jenkins for our continuous integration system to automate running of tests and to perform continuous deployment.
-Digital Playbook#10 Automate testing and deployments
-URL: 
-http://git.triad.local/NorthropGrumman/MedExplorer/tree/master/docs/Software%20Development/Screenshots#jenkins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Our MedExplorer prototype is deployed on a IaaS provider, we selected IBM SoftLayers as our provider.
-Digital Playbook#9 Deploy in a flexible hosting environment
-URL: 
-http://MedExplorer.northropgrumman.com/
-</t>
-  </si>
-  <si>
     <t>Our UX team created a design style guide to provide guidance for the web front end developers. Style guides were updated each sprint with development.
 Digital Playbook#3 Make it simple and intuitive
 URL: 
@@ -227,19 +185,65 @@
 http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Processes/DevOps.md#continuous-deliverydeployment</t>
   </si>
   <si>
-    <t>Our UX team performed a number of usability tests with users and provided feedback to the development staff.
-Once we had some initial features in place, usability tests were run daily.
-Digital Playbook#4 Build the service using agile and iterative practices
-URL: 
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User Centered Design/Research Findings/Focus Group2.pdf
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Research%20Findings/Generative_Research.pdf</t>
-  </si>
-  <si>
     <t>Our MedExplorer prototype was design for multiple platforms including PCs, laptops, tablets, and phones.
 Digital Playbook#2 Address the whole experience, from start to finish
 Digital Playbook#7 Bring in experienced teams
 URL: 
 http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Platform%20Support.md</t>
+  </si>
+  <si>
+    <t>Our User Experience design team interviewed and performed user tests with a number for General Public and Clinician users. The team also met with Northrop Grumman's Clinical Advisory Group as part of our Health Division. Users participated in periodic demonstrations for feedback. Created scenarios and stories. The team gave periodic demonstrations to walk through scenarios and gather feedback. We captured feedback as user stories and added to the backlog for prioritization.
+Digital Playbook#1: Understand what people need
+URL: 
+http://git.triad.local/NorthropGrumman/MedExplorer/tree/master/docs/User%20Centered%20Design/Research%20Findings
+http://git.triad.local/NorthropGrumman/MedExplorer/tree/master/docs/User%20Centered%20Design/Scenarios
+http://git.triad.local/NorthropGrumman/MedExplorer/tree/master/docs/Software%20Development/User-Stories</t>
+  </si>
+  <si>
+    <t>Our User Centered Design approach used a number of techniques and tools, including interviews, focus groups, expectancy tests, generative research, and usability tests.
+Digital Playbook#3 Make it simple and intuitive
+URL: 
+http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Readme.md</t>
+  </si>
+  <si>
+    <t>Our UX team performed a number of usability tests with users and provided feedback to the development staff.
+Once we had some initial features in place, usability tests were run daily.
+Digital Playbook#4 Build the service using agile and iterative practices
+URL: 
+http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Research%20Findings/Focus%20Group2.pdf
+http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Research%20Findings/Generative_Research.pdf</t>
+  </si>
+  <si>
+    <t>Using our Agile framework, which is built upon Scrum, Extreme Programming, and user-centered design techniques, we were able to develop the product in an iterative fashion while receiving regular, timely feedback from users and stakeholders. We conducted an initial sprint 0 as we identified the team and coordinated the infrastructure. Then we used sprint cycles of 5 hours each comprised of sprint planning, execution, and review (demo and retrospective).
+Digital Playbook#4 Build the service using agile and iterative practices
+URL: 
+http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Processes/Readme.md
+http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Readme.md
+http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Iterative%20Development.md
+http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Research%20Findings/Generative_Research.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our MedExplorer used a number for modern, open source technologies, including TwitterBootstrap, AngularJS, NodeJS, ExpressJS, Docker, MongoDB, Jenkins and Zabbix.
+Digital Playbook#8 Choose a modern technology stack
+URL: 
+http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/License.md#open-source-third-party-software-licenses
+http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/Diagrams/MedExplorer_TechnologyStack.png
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our MedExplorer prototype is deployed on a IaaS provider, we selected IBM SoftLayers as our provider.
+Digital Playbook#9 Deploy in a flexible hosting environment
+URL: 
+http://MedExplorer.northropgrumman.com
+http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Screenshots/softlayer.png
+</t>
+  </si>
+  <si>
+    <t>Our development team used Jenkins for our continuous integration system to automate running of tests and to perform continuous deployment.
+Digital Playbook#10 Automate testing and deployments
+URL: 
+http://git.triad.local/NorthropGrumman/MedExplorer/tree/master/docs/Software%20Development/Screenshots#jenkins
+http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Processes/DevOps.md#continuous-integration</t>
   </si>
 </sst>
 </file>
@@ -48724,8 +48728,8 @@
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="41.140625" customWidth="1"/>
-    <col min="3" max="3" width="91" style="13" customWidth="1"/>
-    <col min="4" max="4" width="42.85546875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="126" style="13" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
@@ -48758,7 +48762,7 @@
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
     </row>
-    <row r="2" spans="1:22" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -48766,7 +48770,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="2"/>
@@ -48788,7 +48792,7 @@
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
     </row>
-    <row r="3" spans="1:22" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -48796,7 +48800,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="2"/>
@@ -48818,7 +48822,7 @@
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" ht="141" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" ht="144" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -48826,7 +48830,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="2"/>
@@ -48848,7 +48852,7 @@
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
     </row>
-    <row r="5" spans="1:22" ht="108" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -48856,7 +48860,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="2"/>
@@ -48886,7 +48890,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -48915,7 +48919,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="2"/>
@@ -48937,7 +48941,7 @@
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
     </row>
-    <row r="8" spans="1:22" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" ht="159.94999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -48945,7 +48949,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="2"/>
@@ -48967,7 +48971,7 @@
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
     </row>
-    <row r="9" spans="1:22" ht="111" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" ht="99" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -48975,7 +48979,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="2"/>
@@ -49005,7 +49009,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="2"/>
@@ -49027,7 +49031,7 @@
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
     </row>
-    <row r="11" spans="1:22" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -49035,7 +49039,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="2"/>
@@ -49057,7 +49061,7 @@
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
     </row>
-    <row r="12" spans="1:22" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -49065,7 +49069,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="2"/>
@@ -49095,7 +49099,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="2"/>
@@ -49125,7 +49129,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="2"/>
@@ -49155,7 +49159,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="2"/>
@@ -49185,7 +49189,7 @@
         <v>18</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="2"/>
@@ -49207,7 +49211,7 @@
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
     </row>
-    <row r="17" spans="1:22" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -49215,7 +49219,7 @@
         <v>19</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="2"/>
@@ -49237,7 +49241,7 @@
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
     </row>
-    <row r="18" spans="1:22" ht="155.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" ht="159.94999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -49245,7 +49249,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="2"/>
@@ -49267,7 +49271,7 @@
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
     </row>
-    <row r="19" spans="1:22" ht="78" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -49275,7 +49279,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="2"/>
@@ -49297,7 +49301,7 @@
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
     </row>
-    <row r="20" spans="1:22" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -49305,7 +49309,7 @@
         <v>21</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="2"/>

</xml_diff>